<commit_message>
Created functions that enable finance/bur template automation
</commit_message>
<xml_diff>
--- a/outputs/BURs/tmp_AMC.xlsx
+++ b/outputs/BURs/tmp_AMC.xlsx
@@ -7,21 +7,22 @@
   </bookViews>
   <sheets>
     <sheet name="AMC Aerospace Solutions Divisi" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="AMC Conveyance Solutions Divis" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="AMC IndiaMiddle East" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="AMC Linear Motion Division" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="AMC Micro-Motion Division" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="AMC Motion Control Systems Div" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="AMC Power Management Division" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="AMC Segment Functions" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="AMC Thomson Linear Motion - Ge" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="L1_AMC" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="AMC Autonomous Mobile Solution" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="AMC Conveyance Solutions Divis" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="AMC IndiaMiddle East" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="AMC Linear Motion Division" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="AMC Micro-Motion Division" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="AMC Motion Control Systems Div" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="AMC Power Management Division" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="AMC Segment Functions" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="AMC Thomson Linear Motion - Ge" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="L1_AMC" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve">segment_function</t>
   </si>
@@ -96,6 +97,9 @@
   </si>
   <si>
     <t xml:space="preserve">CY Actual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMC Autonomous Mobile Solutions Division</t>
   </si>
   <si>
     <t xml:space="preserve">AMC Conveyance Solutions Division</t>
@@ -527,55 +531,55 @@
         <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>0.485714285714286</v>
+        <v>0.1165</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0.0094</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6667</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.0229</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7143</v>
+        <v>0.0326</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>0.0181</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5</v>
+        <v>0.0045</v>
       </c>
       <c r="K2" t="n">
-        <v>0.3333</v>
+        <v>0.0132</v>
       </c>
       <c r="L2" t="n">
-        <v>0.3333</v>
+        <v>0.0357</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>0.0043</v>
       </c>
       <c r="N2" t="n">
-        <v>0.3333</v>
+        <v>0.0085</v>
       </c>
       <c r="O2" t="n">
-        <v>0.3333</v>
+        <v>0.0167</v>
       </c>
       <c r="P2" t="n">
-        <v>0.3846</v>
+        <v>0.0298</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>0.0162</v>
       </c>
       <c r="R2" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>0.5</v>
+        <v>0.0039</v>
       </c>
       <c r="T2" t="n">
-        <v>0.5556</v>
+        <v>0.0198</v>
       </c>
     </row>
     <row r="3">
@@ -588,56 +592,54 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="D3"/>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>0.00846</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0.02061</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5</v>
+        <v>0.02934</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>0.01629</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5</v>
+        <v>0.00405</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5</v>
+        <v>0.01188</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5</v>
+        <v>0.03213</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5</v>
+        <v>0.00387</v>
       </c>
       <c r="N3" t="n">
-        <v>0.5</v>
+        <v>0.00765</v>
       </c>
       <c r="O3" t="n">
-        <v>0.5</v>
+        <v>0.01503</v>
       </c>
       <c r="P3" t="n">
-        <v>0.5</v>
+        <v>0.02682</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5</v>
+        <v>0.01458</v>
       </c>
       <c r="R3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5</v>
+        <v>0.00351</v>
       </c>
       <c r="T3" t="n">
-        <v>0.5</v>
+        <v>0.01782</v>
       </c>
     </row>
     <row r="4">
@@ -651,19 +653,19 @@
         <v>24</v>
       </c>
       <c r="D4" t="n">
-        <v>0.266666666666667</v>
+        <v>0.1165</v>
       </c>
       <c r="E4" t="n">
-        <v>0.25</v>
+        <v>0.0094</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3333</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.0229</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2667</v>
+        <v>0.0326</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -677,6 +679,168 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.485714285714286</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.6667</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.7143</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.3333</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.3333</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.3333</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.3333</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.3846</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.5556</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.3333</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.2667</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -765,55 +929,55 @@
         <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>0.626609442060086</v>
+        <v>0.1029</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6316</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7119</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6071</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4737</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.55</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>0.5522</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.625</v>
+        <v>0.0139</v>
       </c>
       <c r="N2" t="n">
-        <v>0.6667</v>
+        <v>0.0299</v>
       </c>
       <c r="O2" t="n">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>0.5538</v>
+        <v>0.0435</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.8824</v>
+        <v>0.0147</v>
       </c>
       <c r="R2" t="n">
-        <v>0.65</v>
+        <v>0.0152</v>
       </c>
       <c r="S2" t="n">
-        <v>0.6</v>
+        <v>0.0308</v>
       </c>
       <c r="T2" t="n">
-        <v>0.7381</v>
+        <v>0.0603</v>
       </c>
     </row>
     <row r="3">
@@ -826,56 +990,54 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="D3"/>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5</v>
+        <v>0.01251</v>
       </c>
       <c r="N3" t="n">
-        <v>0.5</v>
+        <v>0.02691</v>
       </c>
       <c r="O3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0.5</v>
+        <v>0.03915</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5</v>
+        <v>0.01323</v>
       </c>
       <c r="R3" t="n">
-        <v>0.5</v>
+        <v>0.01368</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5</v>
+        <v>0.02772</v>
       </c>
       <c r="T3" t="n">
-        <v>0.5</v>
+        <v>0.05427</v>
       </c>
     </row>
     <row r="4">
@@ -889,19 +1051,19 @@
         <v>24</v>
       </c>
       <c r="D4" t="n">
-        <v>0.611111111111111</v>
+        <v>0.1029</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5357</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7857</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6111</v>
+        <v>0</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -915,6 +1077,516 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1051</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0076</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0057</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0091</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0224</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.0092</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.0107</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.0279</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.0114</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.0106</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.0289</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.0075</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.0094</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" t="n">
+        <v>0.00684</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.00513</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.00819</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.02016</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.00828</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.00963</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0072</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.02511</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0063</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.01026</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.00954</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.02601</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.0081</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.00675</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.00846</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.0234</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1051</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0076</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0057</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0091</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0224</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.626609442060086</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.6316</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.7119</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.6071</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.4737</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.5522</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.6667</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.5538</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.8824</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.7381</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.611111111111111</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.5357</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.7857</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.6111</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1003,55 +1675,55 @@
         <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>0.661016949152542</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6667</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3333</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6667</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7143</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9231</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1064,56 +1736,54 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="D3"/>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1127,19 +1797,19 @@
         <v>24</v>
       </c>
       <c r="D4" t="n">
-        <v>0.466666666666667</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7143</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.4667</v>
+        <v>0</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -1241,28 +1911,56 @@
         <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
+        <v>0.1202</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0097</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0077</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0058</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0232</v>
+      </c>
       <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2"/>
-      <c r="K2"/>
+        <v>0.0154</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.0136</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0059</v>
+      </c>
       <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
+        <v>0.035</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.0061</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.0166</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.0209</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.0432</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.0083</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.0063</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.0041</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.0187</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -1274,57 +1972,255 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="D3"/>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>0.00873</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0.00693</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0.00522</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5</v>
+        <v>0.02088</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>0.01386</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5</v>
+        <v>0.01224</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5</v>
+        <v>0.00531</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5</v>
+        <v>0.0315</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5</v>
+        <v>0.00549</v>
       </c>
       <c r="N3" t="n">
-        <v>0.5</v>
+        <v>0.01494</v>
       </c>
       <c r="O3" t="n">
-        <v>0.5</v>
+        <v>0.01881</v>
       </c>
       <c r="P3" t="n">
-        <v>0.5</v>
+        <v>0.03888</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5</v>
+        <v>0.00747</v>
       </c>
       <c r="R3" t="n">
-        <v>0.5</v>
+        <v>0.00567</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5</v>
+        <v>0.00369</v>
       </c>
       <c r="T3" t="n">
-        <v>0.5</v>
-      </c>
+        <v>0.01683</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1202</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0097</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0077</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0058</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0232</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.661016949152542</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.6667</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.3333</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.6667</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.7143</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.9231</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.466666666666667</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.7143</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.4667</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1413,55 +2309,55 @@
         <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>0.675675675675676</v>
+        <v>0.1587</v>
       </c>
       <c r="E2" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>0.5556</v>
+        <v>0.1429</v>
       </c>
       <c r="O2" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>0.5</v>
+        <v>0.1493</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
         <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>0.8333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1474,56 +2370,54 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="D3"/>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0.5</v>
+        <v>0.12861</v>
       </c>
       <c r="O3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0.5</v>
+        <v>0.13437</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1537,19 +2431,19 @@
         <v>24</v>
       </c>
       <c r="D4" t="n">
-        <v>0.833333333333333</v>
+        <v>0.1587</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3333</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8333</v>
+        <v>0</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -1563,6 +2457,102 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1651,55 +2641,55 @@
         <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>0.65625</v>
+        <v>0.102</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0.0101</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0.004</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.0061</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8889</v>
+        <v>0.0203</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5</v>
+        <v>0.0083</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6</v>
+        <v>0.0146</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>0.0063</v>
       </c>
       <c r="L2" t="n">
-        <v>0.4615</v>
+        <v>0.0292</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>0.0084</v>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>0.0132</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>0.0066</v>
       </c>
       <c r="P2" t="n">
-        <v>0.25</v>
+        <v>0.0281</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>0.0111</v>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
+        <v>0.0067</v>
       </c>
       <c r="S2" t="n">
-        <v>1</v>
+        <v>0.0067</v>
       </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>0.0246</v>
       </c>
     </row>
     <row r="3">
@@ -1712,56 +2702,54 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="D3"/>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>0.00909</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0.0036</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0.00549</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5</v>
+        <v>0.01827</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>0.00747</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5</v>
+        <v>0.01314</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5</v>
+        <v>0.00567</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5</v>
+        <v>0.02628</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5</v>
+        <v>0.00756</v>
       </c>
       <c r="N3" t="n">
-        <v>0.5</v>
+        <v>0.01188</v>
       </c>
       <c r="O3" t="n">
-        <v>0.5</v>
+        <v>0.00594</v>
       </c>
       <c r="P3" t="n">
-        <v>0.5</v>
+        <v>0.02529</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5</v>
+        <v>0.00999</v>
       </c>
       <c r="R3" t="n">
-        <v>0.5</v>
+        <v>0.00603</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5</v>
+        <v>0.00603</v>
       </c>
       <c r="T3" t="n">
-        <v>0.5</v>
+        <v>0.02214</v>
       </c>
     </row>
     <row r="4">
@@ -1775,17 +2763,19 @@
         <v>24</v>
       </c>
       <c r="D4" t="n">
-        <v>0.833333333333333</v>
+        <v>0.102</v>
       </c>
       <c r="E4" t="n">
-        <v>0.75</v>
+        <v>0.0101</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4"/>
+        <v>0.004</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0061</v>
+      </c>
       <c r="H4" t="n">
-        <v>0.8333</v>
+        <v>0.0203</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -1799,6 +2789,168 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.675675675675676</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.5556</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.8333</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.3333</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.8333</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1887,53 +3039,55 @@
         <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>0.813953488372093</v>
+        <v>0.1364</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0.0086</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0.0203</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>0.0087</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0.0376</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8333</v>
+        <v>0.0144</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5</v>
+        <v>0.0203</v>
       </c>
       <c r="K2" t="n">
-        <v>0.6</v>
+        <v>0.0116</v>
       </c>
       <c r="L2" t="n">
-        <v>0.6667</v>
+        <v>0.0463</v>
       </c>
       <c r="M2" t="n">
-        <v>0.4</v>
+        <v>0.0085</v>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>0.0084</v>
       </c>
       <c r="O2" t="n">
-        <v>1</v>
+        <v>0.0028</v>
       </c>
       <c r="P2" t="n">
-        <v>0.625</v>
+        <v>0.0197</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>0.0111</v>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2"/>
+        <v>0.0084</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.0139</v>
+      </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>0.0333</v>
       </c>
     </row>
     <row r="3">
@@ -1946,56 +3100,54 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="D3"/>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>0.00774</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0.01827</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0.00783</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5</v>
+        <v>0.03384</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>0.01296</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5</v>
+        <v>0.01827</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5</v>
+        <v>0.01044</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5</v>
+        <v>0.04167</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5</v>
+        <v>0.00765</v>
       </c>
       <c r="N3" t="n">
-        <v>0.5</v>
+        <v>0.00756</v>
       </c>
       <c r="O3" t="n">
-        <v>0.5</v>
+        <v>0.00252</v>
       </c>
       <c r="P3" t="n">
-        <v>0.5</v>
+        <v>0.01773</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5</v>
+        <v>0.00999</v>
       </c>
       <c r="R3" t="n">
-        <v>0.5</v>
+        <v>0.00756</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5</v>
+        <v>0.01251</v>
       </c>
       <c r="T3" t="n">
-        <v>0.5</v>
+        <v>0.02997</v>
       </c>
     </row>
     <row r="4">
@@ -2009,19 +3161,19 @@
         <v>24</v>
       </c>
       <c r="D4" t="n">
-        <v>0.875</v>
+        <v>0.1364</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0.0086</v>
       </c>
       <c r="F4" t="n">
-        <v>0.75</v>
+        <v>0.0203</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0.0087</v>
       </c>
       <c r="H4" t="n">
-        <v>0.875</v>
+        <v>0.0376</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -2035,6 +3187,166 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.65625</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.8889</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.4615</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7" t="n">
+        <v>0.8333</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2123,45 +3435,55 @@
         <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>0.272727272727273</v>
+        <v>0.0804</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2"/>
+        <v>0.0047</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0012</v>
+      </c>
       <c r="G2" t="n">
-        <v>0.5</v>
+        <v>0.0106</v>
       </c>
       <c r="H2" t="n">
-        <v>0.25</v>
+        <v>0.0165</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5</v>
+        <v>0.0036</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2"/>
+        <v>0.0048</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0073</v>
+      </c>
       <c r="L2" t="n">
-        <v>0.3333</v>
+        <v>0.0157</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2"/>
+        <v>0.0063</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.0076</v>
+      </c>
       <c r="O2" t="n">
-        <v>0.5</v>
+        <v>0.0077</v>
       </c>
       <c r="P2" t="n">
-        <v>0.3333</v>
+        <v>0.0215</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2"/>
-      <c r="S2"/>
+        <v>0.0065</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.0091</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.0118</v>
+      </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>0.0274</v>
       </c>
     </row>
     <row r="3">
@@ -2174,56 +3496,54 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="D3"/>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>0.00423</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0.00108</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0.00954</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5</v>
+        <v>0.01485</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>0.00324</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5</v>
+        <v>0.00432</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5</v>
+        <v>0.00657</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5</v>
+        <v>0.01413</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5</v>
+        <v>0.00567</v>
       </c>
       <c r="N3" t="n">
-        <v>0.5</v>
+        <v>0.00684</v>
       </c>
       <c r="O3" t="n">
-        <v>0.5</v>
+        <v>0.00693</v>
       </c>
       <c r="P3" t="n">
-        <v>0.5</v>
+        <v>0.01935</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5</v>
+        <v>0.00585</v>
       </c>
       <c r="R3" t="n">
-        <v>0.5</v>
+        <v>0.00819</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5</v>
+        <v>0.01062</v>
       </c>
       <c r="T3" t="n">
-        <v>0.5</v>
+        <v>0.02466</v>
       </c>
     </row>
     <row r="4">
@@ -2237,19 +3557,19 @@
         <v>24</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5</v>
+        <v>0.0804</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.0047</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.0012</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0.0106</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5</v>
+        <v>0.0165</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -2263,6 +3583,166 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.813953488372093</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.8333</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.6667</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5"/>
+      <c r="T5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2351,43 +3831,55 @@
         <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>0.333333333333333</v>
+        <v>0.1206</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2"/>
+        <v>0.008</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0078</v>
+      </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.0078</v>
       </c>
       <c r="H2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I2"/>
+        <v>0.0236</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
       <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2"/>
+        <v>0.015</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0148</v>
+      </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>0.0074</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2"/>
+        <v>0.0074</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.0226</v>
+      </c>
       <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2"/>
+        <v>0.0372</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
       <c r="R2" t="n">
-        <v>0.6667</v>
-      </c>
-      <c r="S2"/>
+        <v>0.0147</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.0147</v>
+      </c>
       <c r="T2" t="n">
-        <v>0.6667</v>
+        <v>0.0295</v>
       </c>
     </row>
     <row r="3">
@@ -2400,56 +3892,54 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="D3"/>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>0.0072</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0.00702</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0.00702</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5</v>
+        <v>0.02124</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5</v>
+        <v>0.0135</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5</v>
+        <v>0.01332</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5</v>
+        <v>0.027</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5</v>
+        <v>0.00666</v>
       </c>
       <c r="N3" t="n">
-        <v>0.5</v>
+        <v>0.00666</v>
       </c>
       <c r="O3" t="n">
-        <v>0.5</v>
+        <v>0.02034</v>
       </c>
       <c r="P3" t="n">
-        <v>0.5</v>
+        <v>0.03348</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>0.5</v>
+        <v>0.01323</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5</v>
+        <v>0.01323</v>
       </c>
       <c r="T3" t="n">
-        <v>0.5</v>
+        <v>0.02655</v>
       </c>
     </row>
     <row r="4">
@@ -2463,17 +3953,19 @@
         <v>24</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5</v>
+        <v>0.1206</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5</v>
+        <v>0.008</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G4"/>
+        <v>0.0078</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0078</v>
+      </c>
       <c r="H4" t="n">
-        <v>0.5</v>
+        <v>0.0236</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -2487,6 +3979,158 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.272727272727273</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5"/>
+      <c r="L5" t="n">
+        <v>0.3333</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5"/>
+      <c r="O5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.3333</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2575,30 +4219,38 @@
         <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2"/>
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
       <c r="H2" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2"/>
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M2"/>
-      <c r="N2"/>
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
@@ -2606,12 +4258,16 @@
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
-      </c>
-      <c r="R2"/>
-      <c r="S2"/>
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2624,57 +4280,241 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="D3"/>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0.5</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5"/>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5"/>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5"/>
+      <c r="R5" t="n">
+        <v>0.6667</v>
+      </c>
+      <c r="S5"/>
+      <c r="T5" t="n">
+        <v>0.6667</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reformatted output to match finance
</commit_message>
<xml_diff>
--- a/outputs/BURs/tmp_AMC.xlsx
+++ b/outputs/BURs/tmp_AMC.xlsx
@@ -22,12 +22,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">segment_function</t>
   </si>
   <si>
     <t xml:space="preserve">division_function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cvd</t>
   </si>
   <si>
     <t xml:space="preserve">data_source</t>
@@ -93,13 +96,19 @@
     <t xml:space="preserve">AMC Aerospace Solutions Division</t>
   </si>
   <si>
+    <t xml:space="preserve">Voluntary Turnover Professional</t>
+  </si>
+  <si>
     <t xml:space="preserve">PY Actual</t>
   </si>
   <si>
-    <t xml:space="preserve">Goal</t>
+    <t xml:space="preserve">AOP</t>
   </si>
   <si>
-    <t xml:space="preserve">CY Actual</t>
+    <t xml:space="preserve">Commit/Forecast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal Fill Rate</t>
   </si>
   <si>
     <t xml:space="preserve">AMC Autonomous Mobile Solutions Division</t>
@@ -525,253 +534,290 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.1166</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.0094</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
       <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
         <v>0.0228</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.0324</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.018</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.0045</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.0132</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.0356</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>0.0043</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>0.0085</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>0.0167</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>0.0299</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>0.0163</v>
       </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
       <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
         <v>0.0039</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>0.0199</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>0.1494</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3"/>
-      <c r="E3" t="n">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" t="n">
         <v>0.00846</v>
       </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
       <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
         <v>0.02052</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.02916</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.0162</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.00405</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.01188</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.03204</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>0.00387</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>0.00765</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>0.01503</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>0.02691</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>0.01467</v>
       </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
       <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
         <v>0.00351</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>0.01791</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>0.1494</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="n">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.0498</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.0076</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.0115</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.0192</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.0383</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.0115</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
+      <c r="K4" t="n">
+        <v>0.01245</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.01245</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.03735</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.01245</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.01245</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.01245</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.03735</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.01245</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.01245</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.01245</v>
+      </c>
       <c r="U4" t="n">
+        <v>0.03735</v>
+      </c>
+      <c r="V4" t="n">
         <v>0.1494</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="n">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.485714285714286</v>
       </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
       <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
         <v>0.6667</v>
       </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
       <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.7143</v>
       </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
       <c r="J5" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3333</v>
+        <v>0.5</v>
       </c>
       <c r="L5" t="n">
         <v>0.3333</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>0.3333</v>
       </c>
       <c r="N5" t="n">
-        <v>0.3333</v>
+        <v>1</v>
       </c>
       <c r="O5" t="n">
         <v>0.3333</v>
       </c>
       <c r="P5" t="n">
+        <v>0.3333</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0.3846</v>
       </c>
-      <c r="Q5" t="n">
-        <v>1</v>
-      </c>
       <c r="R5" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S5" t="n">
         <v>0.5</v>
       </c>
       <c r="T5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="U5" t="n">
         <v>0.5556</v>
       </c>
-      <c r="U5"/>
+      <c r="V5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5</v>
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
       <c r="E6" t="n">
         <v>0.5</v>
@@ -821,48 +867,76 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
-      <c r="U6"/>
+      <c r="U6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.25</v>
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
       </c>
       <c r="E7" t="n">
         <v>0.25</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.3077</v>
       </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="V7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -942,23 +1016,26 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.1045</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
@@ -981,47 +1058,50 @@
         <v>0</v>
       </c>
       <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
         <v>0.0141</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>0.0303</v>
       </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
       <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
         <v>0.0441</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>0.0149</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>0.0154</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>0.0312</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>0.0613</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3"/>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3"/>
       <c r="F3" t="n">
         <v>0</v>
       </c>
@@ -1044,139 +1124,170 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
         <v>0.01269</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>0.02727</v>
       </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
       <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
         <v>0.03969</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>0.01341</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>0.01386</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>0.02808</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>0.05517</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
         <v>0.4</v>
       </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
       <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.8511</v>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.25</v>
+      </c>
       <c r="U4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V4" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.5</v>
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5"/>
-      <c r="H5" t="n">
-        <v>0.5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5"/>
       <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5"/>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5"/>
       <c r="L5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M5"/>
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.5</v>
+      </c>
       <c r="N5"/>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
+      <c r="O5"/>
       <c r="P5" t="n">
         <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>1</v>
-      </c>
-      <c r="R5"/>
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
       <c r="S5"/>
-      <c r="T5" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5"/>
+      <c r="T5"/>
+      <c r="U5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5</v>
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
       <c r="E6" t="n">
         <v>0.5</v>
@@ -1226,7 +1337,10 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
-      <c r="U6"/>
+      <c r="U6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1306,253 +1420,290 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.1005</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.0073</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.0055</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.0084</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.0212</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.0088</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.0103</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.0077</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.0268</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>0.0067</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>0.0109</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>0.0102</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>0.0277</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>0.0083</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>0.0072</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>0.0094</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>0.0249</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>0.1098</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3"/>
-      <c r="E3" t="n">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" t="n">
         <v>0.00657</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.00495</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.00756</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.01908</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.00792</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.00927</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.00693</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.02412</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>0.00603</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>0.00981</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>0.00918</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>0.02493</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>0.00747</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>0.00648</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>0.00846</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>0.02241</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>0.1098</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="n">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.0366</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.0087</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.0076</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.0103</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.0266</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.01</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
+      <c r="K4" t="n">
+        <v>0.00915</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.00915</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.02745</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.00915</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.00915</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.00915</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.02745</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.00915</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.00915</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.00915</v>
+      </c>
       <c r="U4" t="n">
+        <v>0.02745</v>
+      </c>
+      <c r="V4" t="n">
         <v>0.1098</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="n">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.626609442060086</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.8</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>0.6316</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>0.6</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>0.7119</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>0.6071</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>0.4737</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>0.55</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>0.5522</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>0.625</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>0.6667</v>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>0.35</v>
       </c>
-      <c r="P5" t="n">
+      <c r="Q5" t="n">
         <v>0.5538</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
         <v>0.8824</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>0.65</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>0.6</v>
       </c>
-      <c r="T5" t="n">
+      <c r="U5" t="n">
         <v>0.7381</v>
       </c>
-      <c r="U5"/>
+      <c r="V5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5</v>
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
       <c r="E6" t="n">
         <v>0.5</v>
@@ -1602,48 +1753,76 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
-      <c r="U6"/>
+      <c r="U6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="n">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.633333333333333</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.5357</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>0.6296</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>0.8</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>0.6286</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.65</v>
       </c>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
+      <c r="K7" t="n">
+        <v>0.633333333333333</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.633333333333333</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.633333333333333</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.633333333333333</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.633333333333333</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.633333333333333</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.633333333333333</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.633333333333333</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.633333333333333</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.633333333333333</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.633333333333333</v>
+      </c>
+      <c r="V7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1723,19 +1902,22 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -1786,23 +1968,26 @@
         <v>0</v>
       </c>
       <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3"/>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3"/>
       <c r="F3" t="n">
         <v>0</v>
       </c>
@@ -1849,21 +2034,24 @@
         <v>0</v>
       </c>
       <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1880,57 +2068,107 @@
       <c r="I4" t="n">
         <v>0</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
       <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5"/>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5"/>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5"/>
       <c r="I5" t="n">
         <v>1</v>
       </c>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="S5"/>
-      <c r="T5"/>
-      <c r="U5"/>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2010,253 +2248,290 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.1021</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.0085</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.0067</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.0034</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.0186</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.0134</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.0118</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.0051</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.0304</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>0.0052</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>0.0142</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>0.0179</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>0.0371</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>0.0071</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>0.0053</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>0.0035</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>0.016</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>0.1332</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3"/>
-      <c r="E3" t="n">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" t="n">
         <v>0.00765</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.00603</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.00306</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.01674</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.01206</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.01062</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.00459</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.02736</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>0.00468</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>0.01278</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>0.01611</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>0.03339</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>0.00639</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>0.00477</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>0.00315</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>0.0144</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>0.1332</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>0.0444</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.0088</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.007</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.016</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.0319</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.0126</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
+      <c r="K4" t="n">
+        <v>0.0111</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.0111</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.0333</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.0111</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.0111</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.0111</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.0333</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.0111</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.0111</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.0111</v>
+      </c>
       <c r="U4" t="n">
+        <v>0.0333</v>
+      </c>
+      <c r="V4" t="n">
         <v>0.1332</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="n">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.661016949152542</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.6667</v>
       </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.3333</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>0.6</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>0.6667</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>0.7143</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>0.65</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>0.9231</v>
       </c>
-      <c r="N5" t="n">
-        <v>1</v>
-      </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0.85</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
         <v>0.8</v>
       </c>
-      <c r="R5" t="n">
-        <v>0.5</v>
-      </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
         <v>0.6</v>
       </c>
-      <c r="U5"/>
+      <c r="V5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5</v>
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
       <c r="E6" t="n">
         <v>0.5</v>
@@ -2306,48 +2581,76 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
-      <c r="U6"/>
+      <c r="U6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>0.55</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.7143</v>
       </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
       <c r="G7" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.4667</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.8</v>
       </c>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
+      <c r="K7" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="V7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2427,23 +2730,26 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.1562</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
@@ -2469,17 +2775,17 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
         <v>0.1429</v>
       </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
       <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
         <v>0.1493</v>
       </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
       <c r="R2" t="n">
         <v>0</v>
       </c>
@@ -2490,23 +2796,26 @@
         <v>0</v>
       </c>
       <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3"/>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3"/>
       <c r="F3" t="n">
         <v>0</v>
       </c>
@@ -2532,17 +2841,17 @@
         <v>0</v>
       </c>
       <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
         <v>0.12861</v>
       </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
       <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
         <v>0.13437</v>
       </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
       <c r="R3" t="n">
         <v>0</v>
       </c>
@@ -2553,21 +2862,24 @@
         <v>0</v>
       </c>
       <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -2584,47 +2896,74 @@
       <c r="I4" t="n">
         <v>0</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
       <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5"/>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5"/>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5"/>
+      <c r="I5"/>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
       <c r="K5"/>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5"/>
+      <c r="L5"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
       <c r="N5"/>
       <c r="O5"/>
       <c r="P5"/>
@@ -2633,19 +2972,20 @@
       <c r="S5"/>
       <c r="T5"/>
       <c r="U5"/>
+      <c r="V5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5</v>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
       <c r="E6" t="n">
         <v>0.5</v>
@@ -2695,7 +3035,10 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
-      <c r="U6"/>
+      <c r="U6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2775,253 +3118,290 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.1034</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.0102</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.0041</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.0062</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.0205</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.0084</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.0148</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.0064</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.0296</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>0.0086</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>0.0134</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>0.0067</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>0.0286</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>0.009</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>0.0068</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>0.0091</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>0.0249</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>0.0921</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3"/>
-      <c r="E3" t="n">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" t="n">
         <v>0.00918</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.00369</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.00558</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.01845</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.00756</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.01332</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.00576</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.02664</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>0.00774</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>0.01206</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>0.00603</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>0.02574</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>0.0081</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>0.00612</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>0.00819</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>0.02241</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>0.0921</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="n">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.0307</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.0101</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.0061</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.0062</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.0225</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.0083</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
+      <c r="K4" t="n">
+        <v>0.007675</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.007675</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.023025</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.007675</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.007675</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.007675</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.023025</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.007675</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.007675</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.007675</v>
+      </c>
       <c r="U4" t="n">
+        <v>0.023025</v>
+      </c>
+      <c r="V4" t="n">
         <v>0.0921</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="n">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.675675675675676</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.75</v>
       </c>
-      <c r="F5" t="n">
-        <v>0.5</v>
-      </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.75</v>
       </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
       <c r="J5" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="n">
         <v>0.8</v>
       </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
       <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
         <v>0.5556</v>
       </c>
-      <c r="O5" t="n">
-        <v>0.5</v>
-      </c>
       <c r="P5" t="n">
         <v>0.5</v>
       </c>
       <c r="Q5" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" t="n">
         <v>0.8333</v>
       </c>
-      <c r="U5"/>
+      <c r="V5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5</v>
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
       <c r="E6" t="n">
         <v>0.5</v>
@@ -3071,48 +3451,76 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
-      <c r="U6"/>
+      <c r="U6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="n">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.733333333333333</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.3333</v>
       </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.8333</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.3333</v>
       </c>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
+      <c r="K7" t="n">
+        <v>0.733333333333333</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.733333333333333</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.733333333333333</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.733333333333333</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.733333333333333</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.733333333333333</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.733333333333333</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.733333333333333</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.733333333333333</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.733333333333333</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.733333333333333</v>
+      </c>
+      <c r="V7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3192,230 +3600,264 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.1352</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.0085</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.0202</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.0086</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.0372</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.0142</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.0201</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.0115</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.0459</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>0.0085</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>0.0084</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>0.0028</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>0.0195</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>0.011</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>0.0083</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>0.0138</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>0.0331</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>0.0756</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3"/>
-      <c r="E3" t="n">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" t="n">
         <v>0.00765</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.01818</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.00774</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.03348</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.01278</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.01809</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.01035</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.04131</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>0.00765</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>0.00756</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>0.00252</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>0.01755</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>0.0099</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>0.00747</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>0.01242</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>0.02979</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>0.0756</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="n">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.0252</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.0028</v>
       </c>
       <c r="F4" t="n">
         <v>0.0028</v>
       </c>
       <c r="G4" t="n">
+        <v>0.0028</v>
+      </c>
+      <c r="H4" t="n">
         <v>0.0084</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.0139</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.0114</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
+      <c r="K4" t="n">
+        <v>0.0063</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.0063</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.0189</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.0063</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.0063</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.0063</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.0189</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.0063</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.0063</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.0063</v>
+      </c>
       <c r="U4" t="n">
+        <v>0.0189</v>
+      </c>
+      <c r="V4" t="n">
         <v>0.0756</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="n">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.65625</v>
       </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.8889</v>
       </c>
-      <c r="I5" t="n">
-        <v>0.5</v>
-      </c>
       <c r="J5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K5" t="n">
         <v>0.6</v>
       </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
       <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
         <v>0.4615</v>
       </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
       <c r="N5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0.25</v>
       </c>
-      <c r="Q5" t="n">
-        <v>1</v>
-      </c>
       <c r="R5" t="n">
         <v>1</v>
       </c>
@@ -3425,20 +3867,23 @@
       <c r="T5" t="n">
         <v>1</v>
       </c>
-      <c r="U5"/>
+      <c r="U5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5</v>
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
       <c r="E6" t="n">
         <v>0.5</v>
@@ -3488,48 +3933,76 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
-      <c r="U6"/>
+      <c r="U6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="n">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.75</v>
       </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.8571</v>
       </c>
-      <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.888888888888889</v>
+      </c>
+      <c r="V7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3609,194 +4082,228 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.0804</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.0047</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.0012</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.0106</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.0165</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.0036</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.0048</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.0073</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.0157</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>0.0063</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>0.0076</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>0.0077</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>0.0215</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>0.0065</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>0.0091</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>0.0118</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>0.0273</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>0.1128</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3"/>
-      <c r="E3" t="n">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" t="n">
         <v>0.00423</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.00108</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.00954</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.01485</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.00324</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.00432</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.00657</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.01413</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>0.00567</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>0.00684</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>0.00693</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>0.01935</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>0.00585</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>0.00819</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>0.01062</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>0.02457</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>0.1128</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="n">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.0376</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.0139</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.0079</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.0063</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.0282</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.0094</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
+      <c r="K4" t="n">
+        <v>0.0094</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.0094</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.0282</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.0094</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.0094</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.0094</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.0282</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.0094</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.0094</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.0094</v>
+      </c>
       <c r="U4" t="n">
+        <v>0.0282</v>
+      </c>
+      <c r="V4" t="n">
         <v>0.1128</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="n">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.813953488372093</v>
       </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
@@ -3807,53 +4314,56 @@
         <v>1</v>
       </c>
       <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
         <v>0.8333</v>
       </c>
-      <c r="J5" t="n">
-        <v>0.5</v>
-      </c>
       <c r="K5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L5" t="n">
         <v>0.6</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>0.6667</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>0.4</v>
       </c>
-      <c r="N5" t="n">
-        <v>1</v>
-      </c>
       <c r="O5" t="n">
         <v>1</v>
       </c>
       <c r="P5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0.625</v>
       </c>
-      <c r="Q5" t="n">
-        <v>1</v>
-      </c>
       <c r="R5" t="n">
         <v>1</v>
       </c>
-      <c r="S5"/>
-      <c r="T5" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5"/>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5"/>
+      <c r="U5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5</v>
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
       <c r="E6" t="n">
         <v>0.5</v>
@@ -3903,48 +4413,76 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
-      <c r="U6"/>
+      <c r="U6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="n">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.842105263157895</v>
       </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
       <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
         <v>0.6667</v>
       </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
       <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.8571</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.8</v>
       </c>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
+      <c r="K7" t="n">
+        <v>0.842105263157895</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.842105263157895</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.842105263157895</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.842105263157895</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.842105263157895</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.842105263157895</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.842105263157895</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.842105263157895</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.842105263157895</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.842105263157895</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.842105263157895</v>
+      </c>
+      <c r="V7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4024,243 +4562,280 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.096</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.0063</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.0062</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.0061</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.0186</v>
       </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
       <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
         <v>0.012</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.0118</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.0239</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.0059</v>
       </c>
       <c r="N2" t="n">
         <v>0.0059</v>
       </c>
       <c r="O2" t="n">
+        <v>0.0059</v>
+      </c>
+      <c r="P2" t="n">
         <v>0.018</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>0.0297</v>
       </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
       <c r="R2" t="n">
-        <v>0.0118</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
         <v>0.0118</v>
       </c>
       <c r="T2" t="n">
+        <v>0.0118</v>
+      </c>
+      <c r="U2" t="n">
         <v>0.0236</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>0.0876</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3"/>
-      <c r="E3" t="n">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" t="n">
         <v>0.00567</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.00558</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.00549</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.01674</v>
       </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
       <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
         <v>0.0108</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.01062</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.02151</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.00531</v>
       </c>
       <c r="N3" t="n">
         <v>0.00531</v>
       </c>
       <c r="O3" t="n">
+        <v>0.00531</v>
+      </c>
+      <c r="P3" t="n">
         <v>0.0162</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>0.02673</v>
       </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
       <c r="R3" t="n">
-        <v>0.01062</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
         <v>0.01062</v>
       </c>
       <c r="T3" t="n">
+        <v>0.01062</v>
+      </c>
+      <c r="U3" t="n">
         <v>0.02124</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>0.0876</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="n">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.0292</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.0058</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.0117</v>
       </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
       <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.0176</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.0116</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
+      <c r="K4" t="n">
+        <v>0.0073</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.0073</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.0219</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.0073</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.0073</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.0073</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.0219</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.0073</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.0073</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.0073</v>
+      </c>
       <c r="U4" t="n">
+        <v>0.0219</v>
+      </c>
+      <c r="V4" t="n">
         <v>0.0876</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="n">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.272727272727273</v>
       </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5"/>
-      <c r="G5" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5"/>
       <c r="H5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.25</v>
       </c>
-      <c r="I5" t="n">
-        <v>0.5</v>
-      </c>
       <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5"/>
-      <c r="L5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5" t="n">
         <v>0.3333</v>
       </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5"/>
-      <c r="O5" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5"/>
       <c r="P5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0.3333</v>
       </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5"/>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
       <c r="S5"/>
-      <c r="T5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5"/>
+      <c r="T5"/>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5</v>
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
       <c r="E6" t="n">
         <v>0.5</v>
@@ -4310,48 +4885,76 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
-      <c r="U6"/>
+      <c r="U6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="n">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.6</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
+        <v>0.5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="V7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4431,19 +5034,22 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -4494,23 +5100,26 @@
         <v>0</v>
       </c>
       <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
         <v>0.1818</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3"/>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3"/>
       <c r="F3" t="n">
         <v>0</v>
       </c>
@@ -4557,115 +5166,146 @@
         <v>0</v>
       </c>
       <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
         <v>0.1818</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="n">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.0606</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
         <v>0.0625</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.0613</v>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.01515</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.01515</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.04545</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.01515</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.01515</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.01515</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.04545</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.01515</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.01515</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.01515</v>
+      </c>
       <c r="U4" t="n">
+        <v>0.04545</v>
+      </c>
+      <c r="V4" t="n">
         <v>0.1818</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="n">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5"/>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5"/>
       <c r="H5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I5"/>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5"/>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5"/>
       <c r="M5" t="n">
         <v>0</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
       </c>
-      <c r="O5"/>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5"/>
-      <c r="R5" t="n">
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5"/>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5"/>
+      <c r="S5" t="n">
         <v>0.6667</v>
       </c>
-      <c r="S5"/>
-      <c r="T5" t="n">
+      <c r="T5"/>
+      <c r="U5" t="n">
         <v>0.6667</v>
       </c>
-      <c r="U5"/>
+      <c r="V5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5</v>
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
       <c r="E6" t="n">
         <v>0.5</v>
@@ -4715,20 +5355,23 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
-      <c r="U6"/>
+      <c r="U6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.5</v>
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
       </c>
       <c r="E7" t="n">
         <v>0.5</v>
@@ -4736,23 +5379,48 @@
       <c r="F7" t="n">
         <v>0.5</v>
       </c>
-      <c r="G7"/>
-      <c r="H7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I7"/>
+      <c r="G7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H7"/>
+      <c r="I7" t="n">
+        <v>0.5</v>
+      </c>
       <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
+      <c r="K7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>